<commit_message>
some testing and some bug fixes
</commit_message>
<xml_diff>
--- a/MonteCarloResultsBUS2TEST.xlsx
+++ b/MonteCarloResultsBUS2TEST.xlsx
@@ -573,31 +573,31 @@
         <v>210</v>
       </c>
       <c r="F2">
-        <v>0.6755725020889205</v>
+        <v>0.5786482193441778</v>
       </c>
       <c r="G2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H2">
-        <v>3.047695498145506</v>
+        <v>2.59096217616796</v>
       </c>
       <c r="I2">
-        <v>0.2216666666666667</v>
+        <v>0.2233333333333333</v>
       </c>
       <c r="J2">
-        <v>179.6076275762049</v>
+        <v>185.6570502286639</v>
       </c>
       <c r="K2">
-        <v>46.55</v>
+        <v>46.9</v>
       </c>
       <c r="L2">
-        <v>141.8702254386733</v>
+        <v>121.5161260622773</v>
       </c>
       <c r="M2">
-        <v>640.0160546105562</v>
+        <v>544.1020569952716</v>
       </c>
       <c r="N2">
-        <v>0.2993460459603416</v>
+        <v>0.3094284170477732</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -617,31 +617,31 @@
         <v>210</v>
       </c>
       <c r="F3">
-        <v>0.9067302374116692</v>
+        <v>0.6580166761854783</v>
       </c>
       <c r="G3">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H3">
-        <v>3.487423990044882</v>
+        <v>2.780352152896387</v>
       </c>
       <c r="I3">
-        <v>0.26</v>
+        <v>0.2366666666666667</v>
       </c>
       <c r="J3">
-        <v>210.0198837628337</v>
+        <v>196.6509103318847</v>
       </c>
       <c r="K3">
-        <v>54.6</v>
+        <v>49.7</v>
       </c>
       <c r="L3">
-        <v>190.4133498564505</v>
+        <v>138.1835019989504</v>
       </c>
       <c r="M3">
-        <v>732.3590379094252</v>
+        <v>583.8739521082413</v>
       </c>
       <c r="N3">
-        <v>0.3500331396047229</v>
+        <v>0.3277515172198078</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -661,31 +661,31 @@
         <v>210</v>
       </c>
       <c r="F4">
-        <v>0.7944082596492344</v>
+        <v>0.9831601997505144</v>
       </c>
       <c r="G4">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="H4">
-        <v>3.479160261237523</v>
+        <v>3.985784593583166</v>
       </c>
       <c r="I4">
-        <v>0.2283333333333333</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="J4">
-        <v>205.3277717707525</v>
+        <v>287.3517655477486</v>
       </c>
       <c r="K4">
-        <v>47.95</v>
+        <v>51.8</v>
       </c>
       <c r="L4">
-        <v>166.8257345263392</v>
+        <v>206.463641947608</v>
       </c>
       <c r="M4">
-        <v>730.6236548598798</v>
+        <v>837.0147646524649</v>
       </c>
       <c r="N4">
-        <v>0.3422129529512542</v>
+        <v>0.4789196092462477</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -705,31 +705,31 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.5270995543688359</v>
+        <v>0.6512537367033345</v>
       </c>
       <c r="G5">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="H5">
-        <v>2.63549777184418</v>
+        <v>2.87317825016177</v>
       </c>
       <c r="I5">
-        <v>0.2</v>
+        <v>0.2266666666666667</v>
       </c>
       <c r="J5">
-        <v>169.2495588000921</v>
+        <v>238.334655591122</v>
       </c>
       <c r="K5">
-        <v>0.2</v>
+        <v>0.2266666666666667</v>
       </c>
       <c r="L5">
-        <v>0.5270995543688359</v>
+        <v>0.6512537367033345</v>
       </c>
       <c r="M5">
-        <v>2.63549777184418</v>
+        <v>2.87317825016177</v>
       </c>
       <c r="N5">
-        <v>0.2820825980001535</v>
+        <v>0.3972244259852034</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -749,31 +749,31 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.5614639041161069</v>
+        <v>0.7736264829465828</v>
       </c>
       <c r="G6">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="H6">
-        <v>2.695026739757313</v>
+        <v>3.136323579513173</v>
       </c>
       <c r="I6">
-        <v>0.2083333333333333</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="J6">
-        <v>164.7187283356711</v>
+        <v>230.3646322165773</v>
       </c>
       <c r="K6">
-        <v>0.2083333333333333</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="L6">
-        <v>0.5614639041161069</v>
+        <v>0.7736264829465828</v>
       </c>
       <c r="M6">
-        <v>2.695026739757313</v>
+        <v>3.136323579513173</v>
       </c>
       <c r="N6">
-        <v>0.2745312138927852</v>
+        <v>0.3839410536942955</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -793,31 +793,31 @@
         <v>10</v>
       </c>
       <c r="F7">
-        <v>0.6141263568802525</v>
+        <v>0.6571696678955942</v>
       </c>
       <c r="G7">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="H7">
-        <v>2.901384363213791</v>
+        <v>2.738206949564976</v>
       </c>
       <c r="I7">
-        <v>0.2116666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="J7">
-        <v>165.0449466649619</v>
+        <v>200.8457690670942</v>
       </c>
       <c r="K7">
-        <v>2.116666666666667</v>
+        <v>2.4</v>
       </c>
       <c r="L7">
-        <v>6.141263568802525</v>
+        <v>6.571696678955941</v>
       </c>
       <c r="M7">
-        <v>29.01384363213791</v>
+        <v>27.38206949564976</v>
       </c>
       <c r="N7">
-        <v>0.2750749111082699</v>
+        <v>0.334742948445157</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -837,31 +837,31 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <v>0.6326065220672403</v>
+        <v>0.6971688234002389</v>
       </c>
       <c r="G8">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="H8">
-        <v>2.875484191214729</v>
+        <v>2.826360094865833</v>
       </c>
       <c r="I8">
-        <v>0.22</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="J8">
-        <v>115.8904371800667</v>
+        <v>135.8568492431152</v>
       </c>
       <c r="K8">
-        <v>2.2</v>
+        <v>2.466666666666667</v>
       </c>
       <c r="L8">
-        <v>6.326065220672403</v>
+        <v>6.971688234002389</v>
       </c>
       <c r="M8">
-        <v>28.75484191214728</v>
+        <v>28.26360094865833</v>
       </c>
       <c r="N8">
-        <v>0.1931507286334444</v>
+        <v>0.2264280820718586</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -881,31 +881,31 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.5873650178355724</v>
+        <v>0.6236740100605981</v>
       </c>
       <c r="G9">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H9">
-        <v>3.203809188194032</v>
+        <v>3.311543416250963</v>
       </c>
       <c r="I9">
-        <v>0.1833333333333333</v>
+        <v>0.1883333333333333</v>
       </c>
       <c r="J9">
-        <v>152.065585738619</v>
+        <v>178.3010857224789</v>
       </c>
       <c r="K9">
-        <v>0.1833333333333333</v>
+        <v>0.1883333333333333</v>
       </c>
       <c r="L9">
-        <v>0.5873650178355724</v>
+        <v>0.6236740100605981</v>
       </c>
       <c r="M9">
-        <v>3.203809188194032</v>
+        <v>3.311543416250963</v>
       </c>
       <c r="N9">
-        <v>0.2534426428976984</v>
+        <v>0.2971684762041314</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -925,31 +925,31 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.41463612921843</v>
+        <v>0.7831049390346055</v>
       </c>
       <c r="G10">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H10">
-        <v>2.261651613918709</v>
+        <v>4.15807932230764</v>
       </c>
       <c r="I10">
-        <v>0.1833333333333333</v>
+        <v>0.1883333333333333</v>
       </c>
       <c r="J10">
-        <v>128.1748567253082</v>
+        <v>266.6544609368764</v>
       </c>
       <c r="K10">
-        <v>0.1833333333333333</v>
+        <v>0.1883333333333333</v>
       </c>
       <c r="L10">
-        <v>0.41463612921843</v>
+        <v>0.7831049390346055</v>
       </c>
       <c r="M10">
-        <v>2.261651613918709</v>
+        <v>4.15807932230764</v>
       </c>
       <c r="N10">
-        <v>0.213624761208847</v>
+        <v>0.4444241015614606</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -969,31 +969,31 @@
         <v>210</v>
       </c>
       <c r="F11">
-        <v>0.6481184082431951</v>
+        <v>0.8083704059571513</v>
       </c>
       <c r="G11">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="H11">
-        <v>2.923842443202384</v>
+        <v>2.993964466507967</v>
       </c>
       <c r="I11">
-        <v>0.2216666666666667</v>
+        <v>0.27</v>
       </c>
       <c r="J11">
-        <v>127.3936461856688</v>
+        <v>172.0179200339518</v>
       </c>
       <c r="K11">
-        <v>46.55</v>
+        <v>56.7</v>
       </c>
       <c r="L11">
-        <v>136.104865731071</v>
+        <v>169.7577852510018</v>
       </c>
       <c r="M11">
-        <v>614.0069130725005</v>
+        <v>628.7325379666731</v>
       </c>
       <c r="N11">
-        <v>0.2123227436427813</v>
+        <v>0.2866965333899197</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1013,31 +1013,31 @@
         <v>210</v>
       </c>
       <c r="F12">
-        <v>0.8307520589309965</v>
+        <v>0.7834668598912301</v>
       </c>
       <c r="G12">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="H12">
-        <v>3.485672974535649</v>
+        <v>2.956478716570679</v>
       </c>
       <c r="I12">
-        <v>0.2383333333333333</v>
+        <v>0.265</v>
       </c>
       <c r="J12">
-        <v>211.7218777614099</v>
+        <v>246.9406585675197</v>
       </c>
       <c r="K12">
-        <v>50.05</v>
+        <v>55.65000000000001</v>
       </c>
       <c r="L12">
-        <v>174.4579323755092</v>
+        <v>164.5280405771583</v>
       </c>
       <c r="M12">
-        <v>731.9913246524864</v>
+        <v>620.8605304798426</v>
       </c>
       <c r="N12">
-        <v>0.3528697962690165</v>
+        <v>0.4115677642791996</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1057,31 +1057,31 @@
         <v>200</v>
       </c>
       <c r="F13">
-        <v>1.033077039556963</v>
+        <v>0.8298225553951707</v>
       </c>
       <c r="G13">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="H13">
-        <v>4.216640977783522</v>
+        <v>3.11183458273189</v>
       </c>
       <c r="I13">
-        <v>0.245</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="J13">
-        <v>227.9181849276904</v>
+        <v>254.0287825301938</v>
       </c>
       <c r="K13">
-        <v>49</v>
+        <v>53.33333333333334</v>
       </c>
       <c r="L13">
-        <v>206.6154079113926</v>
+        <v>165.9645110790341</v>
       </c>
       <c r="M13">
-        <v>843.3281955567044</v>
+        <v>622.3669165463781</v>
       </c>
       <c r="N13">
-        <v>0.3798636415461507</v>
+        <v>0.4233813042169896</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1101,31 +1101,31 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0.7688656840528143</v>
+        <v>0.764627860346198</v>
       </c>
       <c r="G14">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="H14">
-        <v>3.138227281848222</v>
+        <v>2.698686565927758</v>
       </c>
       <c r="I14">
-        <v>0.245</v>
+        <v>0.2833333333333333</v>
       </c>
       <c r="J14">
-        <v>207.5492666912693</v>
+        <v>227.2056409479531</v>
       </c>
       <c r="K14">
-        <v>0.245</v>
+        <v>0.2833333333333333</v>
       </c>
       <c r="L14">
-        <v>0.7688656840528143</v>
+        <v>0.764627860346198</v>
       </c>
       <c r="M14">
-        <v>3.138227281848222</v>
+        <v>2.698686565927758</v>
       </c>
       <c r="N14">
-        <v>0.3459154444854488</v>
+        <v>0.3786760682465886</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1145,31 +1145,31 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0.6940038898482488</v>
+        <v>0.661600576512557</v>
       </c>
       <c r="G15">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="H15">
-        <v>2.932410802175699</v>
+        <v>2.294568473453955</v>
       </c>
       <c r="I15">
-        <v>0.2366666666666667</v>
+        <v>0.2883333333333333</v>
       </c>
       <c r="J15">
-        <v>193.5773941919087</v>
+        <v>210.2484154518459</v>
       </c>
       <c r="K15">
-        <v>0.2366666666666667</v>
+        <v>0.2883333333333333</v>
       </c>
       <c r="L15">
-        <v>0.6940038898482488</v>
+        <v>0.661600576512557</v>
       </c>
       <c r="M15">
-        <v>2.932410802175699</v>
+        <v>2.294568473453955</v>
       </c>
       <c r="N15">
-        <v>0.3226289903198478</v>
+        <v>0.3504140257530765</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1189,31 +1189,31 @@
         <v>10</v>
       </c>
       <c r="F16">
-        <v>0.5800431908713599</v>
+        <v>0.7935588273947127</v>
       </c>
       <c r="G16">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="H16">
-        <v>2.718952457209499</v>
+        <v>2.957362089669737</v>
       </c>
       <c r="I16">
-        <v>0.2133333333333333</v>
+        <v>0.2683333333333333</v>
       </c>
       <c r="J16">
-        <v>120.0734600045116</v>
+        <v>157.7231527787888</v>
       </c>
       <c r="K16">
-        <v>2.133333333333333</v>
+        <v>2.683333333333333</v>
       </c>
       <c r="L16">
-        <v>5.800431908713599</v>
+        <v>7.935588273947127</v>
       </c>
       <c r="M16">
-        <v>27.189524572095</v>
+        <v>29.57362089669737</v>
       </c>
       <c r="N16">
-        <v>0.2001224333408527</v>
+        <v>0.2628719212979814</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1233,31 +1233,31 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>0.9873236301582113</v>
+        <v>0.7328048259383743</v>
       </c>
       <c r="G17">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="H17">
-        <v>3.975799852986086</v>
+        <v>3.186107938862496</v>
       </c>
       <c r="I17">
-        <v>0.2483333333333333</v>
+        <v>0.23</v>
       </c>
       <c r="J17">
-        <v>232.305013465998</v>
+        <v>170.8188476392567</v>
       </c>
       <c r="K17">
-        <v>2.483333333333333</v>
+        <v>2.3</v>
       </c>
       <c r="L17">
-        <v>9.873236301582114</v>
+        <v>7.328048259383743</v>
       </c>
       <c r="M17">
-        <v>39.75799852986086</v>
+        <v>31.86107938862497</v>
       </c>
       <c r="N17">
-        <v>0.38717502244333</v>
+        <v>0.2846980793987611</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1277,31 +1277,31 @@
         <v>200</v>
       </c>
       <c r="F18">
-        <v>1.068039223593384</v>
+        <v>0.6891439518381779</v>
       </c>
       <c r="G18">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="H18">
-        <v>4.85472374360629</v>
+        <v>2.911875852837372</v>
       </c>
       <c r="I18">
-        <v>0.22</v>
+        <v>0.2366666666666667</v>
       </c>
       <c r="J18">
-        <v>243.8880220109039</v>
+        <v>163.2701446236129</v>
       </c>
       <c r="K18">
-        <v>44</v>
+        <v>47.33333333333334</v>
       </c>
       <c r="L18">
-        <v>213.6078447186767</v>
+        <v>137.8287903676356</v>
       </c>
       <c r="M18">
-        <v>970.9447487212581</v>
+        <v>582.3751705674744</v>
       </c>
       <c r="N18">
-        <v>0.4064800366848397</v>
+        <v>0.2721169077060215</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1321,31 +1321,31 @@
         <v>200</v>
       </c>
       <c r="F19">
-        <v>0.6485742856036942</v>
+        <v>0.6058171214429496</v>
       </c>
       <c r="G19">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H19">
-        <v>2.925899032798621</v>
+        <v>2.712613976610222</v>
       </c>
       <c r="I19">
-        <v>0.2216666666666667</v>
+        <v>0.2233333333333333</v>
       </c>
       <c r="J19">
-        <v>189.032023612608</v>
+        <v>174.3352134469874</v>
       </c>
       <c r="K19">
-        <v>44.33333333333334</v>
+        <v>44.66666666666666</v>
       </c>
       <c r="L19">
-        <v>129.7148571207389</v>
+        <v>121.1634242885899</v>
       </c>
       <c r="M19">
-        <v>585.1798065597241</v>
+        <v>542.5227953220444</v>
       </c>
       <c r="N19">
-        <v>0.3150533726876801</v>
+        <v>0.2905586890783123</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1365,31 +1365,31 @@
         <v>200</v>
       </c>
       <c r="F20">
-        <v>0.7084114639498574</v>
+        <v>0.6144837694937428</v>
       </c>
       <c r="G20">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H20">
-        <v>2.993287875844468</v>
+        <v>2.671668563016273</v>
       </c>
       <c r="I20">
-        <v>0.2366666666666667</v>
+        <v>0.23</v>
       </c>
       <c r="J20">
-        <v>199.8532074579925</v>
+        <v>169.6146098924079</v>
       </c>
       <c r="K20">
-        <v>47.33333333333334</v>
+        <v>46</v>
       </c>
       <c r="L20">
-        <v>141.6822927899715</v>
+        <v>122.8967538987486</v>
       </c>
       <c r="M20">
-        <v>598.6575751688936</v>
+        <v>534.3337126032546</v>
       </c>
       <c r="N20">
-        <v>0.3330886790966541</v>
+        <v>0.2826910164873466</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1409,31 +1409,31 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>0.7579998910973083</v>
+        <v>0.6664480209996395</v>
       </c>
       <c r="G21">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H21">
-        <v>3.295651700423079</v>
+        <v>2.961991204442842</v>
       </c>
       <c r="I21">
-        <v>0.23</v>
+        <v>0.225</v>
       </c>
       <c r="J21">
-        <v>186.8191294631245</v>
+        <v>174.9747183350294</v>
       </c>
       <c r="K21">
-        <v>0.23</v>
+        <v>0.225</v>
       </c>
       <c r="L21">
-        <v>0.7579998910973083</v>
+        <v>0.6664480209996395</v>
       </c>
       <c r="M21">
-        <v>3.295651700423079</v>
+        <v>2.961991204442842</v>
       </c>
       <c r="N21">
-        <v>0.3113652157718742</v>
+        <v>0.2916245305583824</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1453,31 +1453,31 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0.6281262805110024</v>
+        <v>0.6906647426133448</v>
       </c>
       <c r="G22">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="H22">
-        <v>2.855119456868193</v>
+        <v>2.79999219978383</v>
       </c>
       <c r="I22">
-        <v>0.22</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="J22">
-        <v>174.6911780743165</v>
+        <v>177.7831288087303</v>
       </c>
       <c r="K22">
-        <v>0.22</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="L22">
-        <v>0.6281262805110024</v>
+        <v>0.6906647426133448</v>
       </c>
       <c r="M22">
-        <v>2.855119456868193</v>
+        <v>2.79999219978383</v>
       </c>
       <c r="N22">
-        <v>0.2911519634571942</v>
+        <v>0.2963052146812172</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1497,31 +1497,31 @@
         <v>10</v>
       </c>
       <c r="F23">
-        <v>0.6839387459166273</v>
+        <v>0.5958149703453176</v>
       </c>
       <c r="G23">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H23">
-        <v>2.97364672137664</v>
+        <v>2.535382852533266</v>
       </c>
       <c r="I23">
-        <v>0.23</v>
+        <v>0.235</v>
       </c>
       <c r="J23">
-        <v>170.5291586184596</v>
+        <v>163.0084991053756</v>
       </c>
       <c r="K23">
-        <v>2.3</v>
+        <v>2.35</v>
       </c>
       <c r="L23">
-        <v>6.839387459166273</v>
+        <v>5.958149703453176</v>
       </c>
       <c r="M23">
-        <v>29.7364672137664</v>
+        <v>25.35382852533267</v>
       </c>
       <c r="N23">
-        <v>0.2842152643640993</v>
+        <v>0.2716808318422927</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1538,16 +1538,16 @@
         <v>1908</v>
       </c>
       <c r="K24">
-        <v>0.2323410202655486</v>
+        <v>0.2443273934311671</v>
       </c>
       <c r="L24">
-        <v>0.8077633413410945</v>
+        <v>0.7278211462211549</v>
       </c>
       <c r="M24">
-        <v>3.476628192550248</v>
+        <v>2.978876563942061</v>
       </c>
       <c r="N24">
-        <v>6.625751598367286</v>
+        <v>7.303311518412024</v>
       </c>
       <c r="O24">
         <v>600</v>
@@ -1556,7 +1556,7 @@
         <v>0.05</v>
       </c>
       <c r="Q24">
-        <v>0.04121623419978665</v>
+        <v>0.04216931777475056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>